<commit_message>
LITE-28133 Add capability to upload price file for a Marketplace in a Hub
</commit_message>
<xml_diff>
--- a/tests/fixtures/Sweet_Pies_v2.xlsx
+++ b/tests/fixtures/Sweet_Pies_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmondal00/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmondal00/projects/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DBAE7A-EA91-E345-BAB7-D842D74A03D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FBD898-E9C5-C74E-9A63-913BAA10D06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,14 @@
     <sheet name="Resources" sheetId="2" r:id="rId4"/>
     <sheet name="PlanPeriods" sheetId="4" r:id="rId5"/>
     <sheet name="ResourceRates" sheetId="6" r:id="rId6"/>
-    <sheet name="OpUnitServicePlans-deleted" sheetId="5" r:id="rId7"/>
+    <sheet name="OpUnitServicePlans" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="228">
   <si>
     <t/>
   </si>
@@ -670,9 +670,6 @@
     <t>US</t>
   </si>
   <si>
-    <t>Reseller ST L2</t>
-  </si>
-  <si>
     <t>Resource</t>
   </si>
   <si>
@@ -710,13 +707,16 @@
   </si>
   <si>
     <t>DisplayInCCP</t>
+  </si>
+  <si>
+    <t>Reseller US L2 ST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -752,6 +752,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -773,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -787,6 +793,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2322,7 +2329,7 @@
   <dimension ref="A1:AZ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+      <selection activeCell="AP26" sqref="AP26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2344,7 +2351,7 @@
     <col min="30" max="30" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.6640625" customWidth="1"/>
     <col min="34" max="34" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="16.5" bestFit="1" customWidth="1"/>
@@ -2619,12 +2626,8 @@
         <v>4</v>
       </c>
       <c r="AG2"/>
-      <c r="AH2">
-        <v>1</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>197</v>
-      </c>
+      <c r="AH2"/>
+      <c r="AI2"/>
       <c r="AJ2" t="s">
         <v>199</v>
       </c>
@@ -2645,7 +2648,7 @@
         <v>201</v>
       </c>
       <c r="AS2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AT2" t="s">
         <v>44</v>
@@ -2764,12 +2767,8 @@
         <v>4</v>
       </c>
       <c r="AG3"/>
-      <c r="AH3">
-        <v>1</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>197</v>
-      </c>
+      <c r="AH3"/>
+      <c r="AI3"/>
       <c r="AJ3" t="s">
         <v>199</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>201</v>
       </c>
       <c r="AS3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AT3" t="s">
         <v>44</v>
@@ -2909,12 +2908,8 @@
         <v>4</v>
       </c>
       <c r="AG4"/>
-      <c r="AH4">
-        <v>1</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>197</v>
-      </c>
+      <c r="AH4"/>
+      <c r="AI4"/>
       <c r="AJ4" t="s">
         <v>199</v>
       </c>
@@ -2935,7 +2930,7 @@
         <v>201</v>
       </c>
       <c r="AS4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AT4" t="s">
         <v>44</v>
@@ -3151,10 +3146,10 @@
         <v>96</v>
       </c>
       <c r="D1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" t="s">
         <v>226</v>
-      </c>
-      <c r="E1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3501,40 +3496,40 @@
         <v>203</v>
       </c>
       <c r="B1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" t="s">
         <v>215</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>216</v>
-      </c>
-      <c r="D1" t="s">
-        <v>217</v>
       </c>
       <c r="E1" t="s">
         <v>56</v>
       </c>
       <c r="F1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" t="s">
         <v>218</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>219</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>220</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>221</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>222</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>223</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>224</v>
-      </c>
-      <c r="M1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3715,7 +3710,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3740,7 +3735,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>213</v>
       </c>
@@ -3748,13 +3743,13 @@
         <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -3762,13 +3757,13 @@
         <v>150</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -3776,10 +3771,10 @@
         <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>214</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>